<commit_message>
removed an unused directory
</commit_message>
<xml_diff>
--- a/useCasesSHS.xlsx
+++ b/useCasesSHS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Defaut\Documents\A_Cours\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgekoutsaris/Desktop/UNIVERSITY/Concordia/SEMESTERS/FALL 2020/SOEN 343/SOEN 343 PROJECT/soen343_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9B365C9-D9FC-4ECB-9FE1-0197B9E6B333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266C4CEE-B555-4A43-93C6-070CCF5F6417}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20175" yWindow="1710" windowWidth="17280" windowHeight="8970" xr2:uid="{5797803E-4189-4FD0-96CB-DECF01A43E99}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16840" xr2:uid="{5797803E-4189-4FD0-96CB-DECF01A43E99}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -737,20 +737,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2488A930-D336-41A3-85A3-BEF5FBEF80B1}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B2:C90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
-    <col min="3" max="3" width="61.21875" customWidth="1"/>
+    <col min="3" max="3" width="61.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -758,7 +761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -766,7 +769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -774,7 +777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
@@ -782,7 +785,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
@@ -790,7 +793,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" ht="48" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
@@ -798,7 +801,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
@@ -806,7 +809,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
@@ -814,7 +817,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
@@ -822,7 +825,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>2</v>
       </c>
@@ -830,7 +833,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
@@ -838,7 +841,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B14" s="6" t="s">
         <v>6</v>
       </c>
@@ -846,7 +849,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
         <v>8</v>
       </c>
@@ -854,7 +857,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" ht="112" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
@@ -862,7 +865,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>12</v>
       </c>
@@ -870,7 +873,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="9" t="s">
         <v>14</v>
       </c>
@@ -878,7 +881,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>0</v>
       </c>
@@ -886,7 +889,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>2</v>
       </c>
@@ -894,7 +897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>4</v>
       </c>
@@ -902,7 +905,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="6" t="s">
         <v>6</v>
       </c>
@@ -910,7 +913,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
         <v>8</v>
       </c>
@@ -918,7 +921,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" ht="144" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>10</v>
       </c>
@@ -926,7 +929,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>12</v>
       </c>
@@ -934,7 +937,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
         <v>14</v>
       </c>
@@ -942,7 +945,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>0</v>
       </c>
@@ -950,7 +953,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
         <v>2</v>
       </c>
@@ -958,7 +961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
         <v>4</v>
       </c>
@@ -966,7 +969,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B32" s="6" t="s">
         <v>6</v>
       </c>
@@ -974,7 +977,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B33" s="6" t="s">
         <v>8</v>
       </c>
@@ -982,7 +985,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" ht="80" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
         <v>10</v>
       </c>
@@ -990,7 +993,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
         <v>12</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B36" s="3" t="s">
         <v>14</v>
       </c>
@@ -1006,7 +1009,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>0</v>
       </c>
@@ -1014,7 +1017,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
         <v>2</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
         <v>4</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
         <v>6</v>
       </c>
@@ -1038,7 +1041,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
         <v>8</v>
       </c>
@@ -1046,7 +1049,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:3" ht="48" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
         <v>10</v>
       </c>
@@ -1054,7 +1057,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
         <v>12</v>
       </c>
@@ -1062,7 +1065,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
         <v>14</v>
       </c>
@@ -1070,7 +1073,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>0</v>
       </c>
@@ -1078,7 +1081,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B48" s="3" t="s">
         <v>2</v>
       </c>
@@ -1086,7 +1089,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" s="3" t="s">
         <v>4</v>
       </c>
@@ -1094,7 +1097,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" s="3" t="s">
         <v>6</v>
       </c>
@@ -1102,7 +1105,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B51" s="3" t="s">
         <v>8</v>
       </c>
@@ -1110,7 +1113,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="52" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:3" ht="48" x14ac:dyDescent="0.2">
       <c r="B52" s="3" t="s">
         <v>10</v>
       </c>
@@ -1118,7 +1121,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B53" s="3" t="s">
         <v>12</v>
       </c>
@@ -1126,7 +1129,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B54" s="3" t="s">
         <v>14</v>
       </c>
@@ -1134,7 +1137,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
         <v>0</v>
       </c>
@@ -1142,7 +1145,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B57" s="3" t="s">
         <v>2</v>
       </c>
@@ -1150,7 +1153,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B58" s="3" t="s">
         <v>4</v>
       </c>
@@ -1158,7 +1161,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B59" s="3" t="s">
         <v>6</v>
       </c>
@@ -1166,7 +1169,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B60" s="3" t="s">
         <v>8</v>
       </c>
@@ -1174,7 +1177,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:3" ht="48" x14ac:dyDescent="0.2">
       <c r="B61" s="3" t="s">
         <v>10</v>
       </c>
@@ -1182,7 +1185,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B62" s="3" t="s">
         <v>12</v>
       </c>
@@ -1190,7 +1193,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B63" s="3" t="s">
         <v>14</v>
       </c>
@@ -1198,7 +1201,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B65" s="1" t="s">
         <v>0</v>
       </c>
@@ -1206,7 +1209,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B66" s="3" t="s">
         <v>2</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B67" s="3" t="s">
         <v>4</v>
       </c>
@@ -1222,7 +1225,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B68" s="3" t="s">
         <v>6</v>
       </c>
@@ -1230,7 +1233,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B69" s="3" t="s">
         <v>8</v>
       </c>
@@ -1238,7 +1241,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:3" ht="48" x14ac:dyDescent="0.2">
       <c r="B70" s="3" t="s">
         <v>10</v>
       </c>
@@ -1246,7 +1249,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="71" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:3" ht="32" x14ac:dyDescent="0.2">
       <c r="B71" s="3" t="s">
         <v>12</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B72" s="3" t="s">
         <v>14</v>
       </c>
@@ -1262,7 +1265,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B74" s="1" t="s">
         <v>0</v>
       </c>
@@ -1270,7 +1273,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B75" s="3" t="s">
         <v>2</v>
       </c>
@@ -1278,7 +1281,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B76" s="3" t="s">
         <v>4</v>
       </c>
@@ -1286,7 +1289,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B77" s="3" t="s">
         <v>6</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B78" s="3" t="s">
         <v>8</v>
       </c>
@@ -1302,7 +1305,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="79" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:3" ht="48" x14ac:dyDescent="0.2">
       <c r="B79" s="3" t="s">
         <v>10</v>
       </c>
@@ -1310,7 +1313,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B80" s="3" t="s">
         <v>12</v>
       </c>
@@ -1318,7 +1321,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B81" s="3" t="s">
         <v>14</v>
       </c>
@@ -1326,7 +1329,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B83" s="1" t="s">
         <v>0</v>
       </c>
@@ -1334,7 +1337,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B84" s="3" t="s">
         <v>2</v>
       </c>
@@ -1342,7 +1345,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B85" s="3" t="s">
         <v>4</v>
       </c>
@@ -1350,7 +1353,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B86" s="3" t="s">
         <v>6</v>
       </c>
@@ -1358,7 +1361,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B87" s="3" t="s">
         <v>8</v>
       </c>
@@ -1366,7 +1369,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="88" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:3" ht="48" x14ac:dyDescent="0.2">
       <c r="B88" s="3" t="s">
         <v>10</v>
       </c>
@@ -1374,7 +1377,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B89" s="3" t="s">
         <v>12</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B90" s="3" t="s">
         <v>14</v>
       </c>
@@ -1392,5 +1395,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="38" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>